<commit_message>
Proper Gantt Chart created and added to Portfolio
</commit_message>
<xml_diff>
--- a/Gantt Chart.xlsx
+++ b/Gantt Chart.xlsx
@@ -233,100 +233,97 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$31</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>Task</c:v>
+                  <c:v>Define the problem</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Define the problem</c:v>
+                  <c:v>Proposal</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Proposal</c:v>
+                  <c:v>Identification of the Problem</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Identification of the Problem</c:v>
+                  <c:v>Ideas</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Ideas</c:v>
+                  <c:v>Requirements</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Requirements</c:v>
+                  <c:v>Understanding the Problem</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Understanding the Problem</c:v>
+                  <c:v>Storyboard</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Storyboard</c:v>
+                  <c:v>Context Diagram</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Context Diagram</c:v>
+                  <c:v>Feasibility Study</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Feasibility Study</c:v>
+                  <c:v>Social and Ethical Issues</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Social and Ethical Issues</c:v>
+                  <c:v>Plan and Design</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Plan and Design</c:v>
+                  <c:v>Data Flow Diagram</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Data Flow Diagram</c:v>
+                  <c:v>Systems Flowchart</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Systems Flowchart</c:v>
+                  <c:v>Specifications</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Specifications</c:v>
+                  <c:v>Data Dictionary</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Data Dictionary</c:v>
+                  <c:v>Algorithms</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Algorithms</c:v>
+                  <c:v>Test Data</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Test Data</c:v>
+                  <c:v>IPO Chart</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>IPO Chart</c:v>
+                  <c:v>Window Design</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Window Design</c:v>
+                  <c:v>Feedback</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Feedback</c:v>
+                  <c:v>Implementation</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Implementation</c:v>
+                  <c:v>Implementing the program</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Implementing the program</c:v>
+                  <c:v>User Documentation</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>User Documentation</c:v>
+                  <c:v>Evaluation</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Evaluation</c:v>
+                  <c:v>Testing with test data</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Testing with test data</c:v>
+                  <c:v>Testing with other users</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Testing with other users</c:v>
+                  <c:v>Testing with school computers</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Testing with school computers</c:v>
+                  <c:v>Maintenance</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Maintenance</c:v>
+                  <c:v>Altering the program</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Altering the program</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Social and Ethical Issues</c:v>
                 </c:pt>
               </c:strCache>
@@ -433,7 +430,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5D85-4E33-861B-DCEC0C51851C}"/>
+              <c16:uniqueId val="{00000000-D515-4EF3-82C2-11D3D90A68F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -453,102 +450,194 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-D515-4EF3-82C2-11D3D90A68F5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-D515-4EF3-82C2-11D3D90A68F5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-D515-4EF3-82C2-11D3D90A68F5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000006-D515-4EF3-82C2-11D3D90A68F5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-D515-4EF3-82C2-11D3D90A68F5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$1:$A$31</c:f>
+              <c:f>Sheet1!$A$2:$A$31</c:f>
               <c:strCache>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>Task</c:v>
+                  <c:v>Define the problem</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Define the problem</c:v>
+                  <c:v>Proposal</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Proposal</c:v>
+                  <c:v>Identification of the Problem</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Identification of the Problem</c:v>
+                  <c:v>Ideas</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Ideas</c:v>
+                  <c:v>Requirements</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Requirements</c:v>
+                  <c:v>Understanding the Problem</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Understanding the Problem</c:v>
+                  <c:v>Storyboard</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Storyboard</c:v>
+                  <c:v>Context Diagram</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Context Diagram</c:v>
+                  <c:v>Feasibility Study</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>Feasibility Study</c:v>
+                  <c:v>Social and Ethical Issues</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Social and Ethical Issues</c:v>
+                  <c:v>Plan and Design</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>Plan and Design</c:v>
+                  <c:v>Data Flow Diagram</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Data Flow Diagram</c:v>
+                  <c:v>Systems Flowchart</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Systems Flowchart</c:v>
+                  <c:v>Specifications</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Specifications</c:v>
+                  <c:v>Data Dictionary</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Data Dictionary</c:v>
+                  <c:v>Algorithms</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>Algorithms</c:v>
+                  <c:v>Test Data</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Test Data</c:v>
+                  <c:v>IPO Chart</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>IPO Chart</c:v>
+                  <c:v>Window Design</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>Window Design</c:v>
+                  <c:v>Feedback</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>Feedback</c:v>
+                  <c:v>Implementation</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>Implementation</c:v>
+                  <c:v>Implementing the program</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>Implementing the program</c:v>
+                  <c:v>User Documentation</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>User Documentation</c:v>
+                  <c:v>Evaluation</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>Evaluation</c:v>
+                  <c:v>Testing with test data</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>Testing with test data</c:v>
+                  <c:v>Testing with other users</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>Testing with other users</c:v>
+                  <c:v>Testing with school computers</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>Testing with school computers</c:v>
+                  <c:v>Maintenance</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>Maintenance</c:v>
+                  <c:v>Altering the program</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>Altering the program</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>Social and Ethical Issues</c:v>
                 </c:pt>
               </c:strCache>
@@ -556,63 +645,63 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$31</c:f>
+              <c:f>Sheet1!$C$2:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1</c:v>
@@ -621,36 +710,33 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
@@ -658,7 +744,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5D85-4E33-861B-DCEC0C51851C}"/>
+              <c16:uniqueId val="{00000001-D515-4EF3-82C2-11D3D90A68F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -672,11 +758,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="103858344"/>
-        <c:axId val="103857360"/>
+        <c:axId val="473326232"/>
+        <c:axId val="473327544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="103858344"/>
+        <c:axId val="473326232"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -690,8 +776,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:alpha val="80000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -718,7 +805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103857360"/>
+        <c:crossAx val="473327544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -726,9 +813,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="103857360"/>
+        <c:axId val="473327544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="42893"/>
           <c:min val="42688"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -778,7 +866,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="103858344"/>
+        <c:crossAx val="473326232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1376,23 +1464,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>819151</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>234949</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AC2D265-A6C0-498F-8D9B-75B14D6528C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{873C6EC3-2EED-4703-ABE7-A254E40E949A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1712,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>